<commit_message>
Updated Project Management Sheet
</commit_message>
<xml_diff>
--- a/Tasks_for_Pegasys.xlsx
+++ b/Tasks_for_Pegasys.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14660" tabRatio="573" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14660" tabRatio="573"/>
   </bookViews>
   <sheets>
     <sheet name="Table of Contents" sheetId="1" r:id="rId1"/>
@@ -630,7 +630,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
@@ -689,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
@@ -729,7 +731,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="36" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>45</v>
       </c>
     </row>
@@ -862,7 +864,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
@@ -896,7 +898,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="36" customHeight="1">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>22</v>
       </c>
     </row>
@@ -918,9 +920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -984,9 +984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -1041,7 +1039,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
@@ -1094,10 +1092,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="72" customHeight="1">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C6" s="3" t="s">

</xml_diff>

<commit_message>
Trying to remove node modules from remote
</commit_message>
<xml_diff>
--- a/Tasks_for_Pegasys.xlsx
+++ b/Tasks_for_Pegasys.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14660" tabRatio="573" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="20" windowWidth="25600" windowHeight="14660" tabRatio="573" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Table of Contents" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="48">
   <si>
     <t>Google API Logic</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>Deploy on Heruko</t>
+  </si>
+  <si>
+    <t>FYI: run "mongod --dbpath ." from database directory to run mongo server</t>
   </si>
 </sst>
 </file>
@@ -259,7 +262,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="17"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="17" applyAlignment="1">
@@ -279,6 +282,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="18">
@@ -689,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
@@ -861,13 +867,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="16384" width="18" style="3"/>
+    <col min="1" max="5" width="18" style="3"/>
+    <col min="6" max="6" width="32.6640625" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="18" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="36" customHeight="1">
@@ -890,15 +898,19 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="36" customHeight="1">
+    <row r="3" spans="1:6" ht="116" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>12</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="36" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="F4" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
updating, trying to pull from origin master
</commit_message>
<xml_diff>
--- a/Tasks_for_Pegasys.xlsx
+++ b/Tasks_for_Pegasys.xlsx
@@ -168,7 +168,7 @@
     <t>Deploy on Heruko</t>
   </si>
   <si>
-    <t>FYI: run "mongod --dbpath ." from database directory to run mongo server</t>
+    <t>FYI: run "mongod --dbpath ." from database directory to run mongo server. Mongo server must be started before Mongo shell (command: "mongo").</t>
   </si>
 </sst>
 </file>
@@ -868,7 +868,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
starting MongoDB requests refactoring
</commit_message>
<xml_diff>
--- a/Tasks_for_Pegasys.xlsx
+++ b/Tasks_for_Pegasys.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="20" windowWidth="25600" windowHeight="14660" tabRatio="573" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="20" windowWidth="25600" windowHeight="14660" tabRatio="573"/>
   </bookViews>
   <sheets>
     <sheet name="Table of Contents" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="50">
   <si>
     <t>Google API Logic</t>
   </si>
@@ -168,7 +168,13 @@
     <t>Deploy on Heruko</t>
   </si>
   <si>
-    <t>FYI: run "mongod --dbpath ." from database directory to run mongo server. Mongo server must be started before Mongo shell (command: "mongo").</t>
+    <t>X</t>
+  </si>
+  <si>
+    <t>server written to support heroku deployment</t>
+  </si>
+  <si>
+    <t>FYI: run "mongod --dbpath ." from database directory to run local mongo server. Mongo server must be started before Mongo shell (command: "mongo").</t>
   </si>
 </sst>
 </file>
@@ -636,7 +642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
@@ -696,7 +702,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
@@ -733,10 +739,16 @@
       <c r="A4" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="36" customHeight="1">
+      <c r="F4" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="77" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>45</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="36" customHeight="1">
@@ -867,7 +879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -903,7 +915,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="36" customHeight="1">

</xml_diff>

<commit_message>
created endPointsRouter + more debugging
</commit_message>
<xml_diff>
--- a/Tasks_for_Pegasys.xlsx
+++ b/Tasks_for_Pegasys.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="20" windowWidth="25600" windowHeight="14660" tabRatio="573"/>
+    <workbookView xWindow="0" yWindow="20" windowWidth="25600" windowHeight="14660" tabRatio="573" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Table of Contents" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="50">
   <si>
     <t>Google API Logic</t>
   </si>
@@ -165,16 +165,16 @@
     <t>Add support for Heroku</t>
   </si>
   <si>
-    <t>Deploy on Heruko</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>server written to support heroku deployment</t>
   </si>
   <si>
     <t>FYI: run "mongod --dbpath ." from database directory to run local mongo server. Mongo server must be started before Mongo shell (command: "mongo").</t>
+  </si>
+  <si>
+    <t>Deploy on Heroku</t>
+  </si>
+  <si>
+    <t>Complete URL paths are a concatenation of the pathname extensions from the middleware file and the routes file</t>
   </si>
 </sst>
 </file>
@@ -268,7 +268,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="17"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="17" applyAlignment="1">
@@ -288,9 +288,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="18">
@@ -642,7 +639,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
@@ -702,7 +701,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
@@ -735,12 +734,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="36" customHeight="1">
+    <row r="4" spans="1:6" ht="135" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="77" customHeight="1">
@@ -748,12 +747,12 @@
         <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="36" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -879,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
@@ -915,14 +914,16 @@
         <v>12</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="36" customHeight="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="119" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
tailored README.md for our app; updated project task manager spreadsheet
</commit_message>
<xml_diff>
--- a/Tasks_for_Pegasys.xlsx
+++ b/Tasks_for_Pegasys.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
   <si>
     <t>Google API Logic</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>Complete URL paths are a concatenation of the pathname extensions from the middleware file and the routes file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reminders: *every object POSTed to /api/profile or /api/createtrip/setroute  must specify the user's driver status or it will default to false; </t>
   </si>
 </sst>
 </file>
@@ -701,7 +704,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
@@ -879,7 +882,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
@@ -909,9 +912,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="116" customHeight="1">
+    <row r="3" spans="1:6" ht="155" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>47</v>

</xml_diff>